<commit_message>
added view to finger coverage sensor
</commit_message>
<xml_diff>
--- a/FingerCoverage.xlsx
+++ b/FingerCoverage.xlsx
@@ -650,11 +650,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2125687480"/>
-        <c:axId val="-2125788200"/>
+        <c:axId val="2116814328"/>
+        <c:axId val="2116821464"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2125687480"/>
+        <c:axId val="2116814328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -695,12 +695,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2125788200"/>
+        <c:crossAx val="2116821464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2125788200"/>
+        <c:axId val="2116821464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -735,7 +735,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2125687480"/>
+        <c:crossAx val="2116814328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1114,10 +1114,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="A31" sqref="A31:B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1616,6 +1616,90 @@
         <v>41.836759887397001</v>
       </c>
     </row>
+    <row r="26" spans="1:6">
+      <c r="A26">
+        <v>77.6866324266975</v>
+      </c>
+      <c r="B26">
+        <v>14.2141435365739</v>
+      </c>
+      <c r="E26">
+        <v>149.84942756558601</v>
+      </c>
+      <c r="F26">
+        <v>39.3217511920775</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27">
+        <v>69.7821720679012</v>
+      </c>
+      <c r="B27">
+        <v>13.645315012376701</v>
+      </c>
+      <c r="E27">
+        <v>151.11446421682101</v>
+      </c>
+      <c r="F27">
+        <v>40.128415075295003</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28">
+        <v>67.395091145833305</v>
+      </c>
+      <c r="B28">
+        <v>14.101743942263001</v>
+      </c>
+      <c r="E28">
+        <v>164.045675636574</v>
+      </c>
+      <c r="F28">
+        <v>43.324295036000201</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29">
+        <v>92.324103491512304</v>
+      </c>
+      <c r="B29">
+        <v>10.6358429078933</v>
+      </c>
+      <c r="E29">
+        <v>247.413308738426</v>
+      </c>
+      <c r="F29">
+        <v>13.501595200559599</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30">
+        <v>86.729440104166699</v>
+      </c>
+      <c r="B30">
+        <v>17.5385200503747</v>
+      </c>
+      <c r="E30">
+        <v>255</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31">
+        <v>92.0986593364198</v>
+      </c>
+      <c r="B31">
+        <v>17.485573008820701</v>
+      </c>
+      <c r="E31">
+        <v>153.06617621527801</v>
+      </c>
+      <c r="F31">
+        <v>81.889863767423194</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:B1"/>
@@ -1623,7 +1707,6 @@
     <mergeCell ref="E1:F1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>